<commit_message>
Updated @Batchdata_Template.xlsx, column fields in Conversation that we are losing in the pipeline the names of both email and phone for all 10 records resulting in 40 records. This total being added to @Batchdata_Template.xlsx. Up next is ensuring that the template is actually followed. Currently, none of the E-Corp first number of columns are being brought in to either the upload or complete output files, so we’ve got to make sure they’re in there. Hopefully without losing functionality if the scripts are separate, those being the ETL and the BatchData scripts pipelines.
</commit_message>
<xml_diff>
--- a/Batchdata_Template.xlsx
+++ b/Batchdata_Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrettsullivan/Desktop/BHRF/Data_Recourses/LANDSCRAPE/adhs-restore-28-Jul-2025 copy/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrettsullivan/Desktop/BHRF/Data_Recourses/LANDSCRAPE/adhs-working/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C7CE35-9D45-554C-AC81-3D402E11649A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28AA11F1-2D83-F140-9505-FD3E8EB6704B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18120" windowHeight="22400" xr2:uid="{ED9AA6DF-8EAD-9141-9DC3-5FD70562401F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{ED9AA6DF-8EAD-9141-9DC3-5FD70562401F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="165">
   <si>
     <t>ECORP_INDEX_#</t>
   </si>
@@ -411,6 +411,126 @@
   </si>
   <si>
     <t>BD_STAGES_APPLIED</t>
+  </si>
+  <si>
+    <t>BD_PHONE_1_FIRST</t>
+  </si>
+  <si>
+    <t>BD_PHONE_1_LAST</t>
+  </si>
+  <si>
+    <t>BD_EMAIL_1_FIRST</t>
+  </si>
+  <si>
+    <t>BD_EMAIL_1_LAST</t>
+  </si>
+  <si>
+    <t>BD_EMAIL_10_FIRST</t>
+  </si>
+  <si>
+    <t>BD_EMAIL_10_LAST</t>
+  </si>
+  <si>
+    <t>BD_EMAIL_9_FIRST</t>
+  </si>
+  <si>
+    <t>BD_EMAIL_9_LAST</t>
+  </si>
+  <si>
+    <t>BD_EMAIL_8_FIRST</t>
+  </si>
+  <si>
+    <t>BD_EMAIL_8_LAST</t>
+  </si>
+  <si>
+    <t>BD_EMAIL_7_LAST</t>
+  </si>
+  <si>
+    <t>BD_EMAIL_7_FIRST</t>
+  </si>
+  <si>
+    <t>BD_EMAIL_6_FIRST</t>
+  </si>
+  <si>
+    <t>BD_EMAIL_6_LAST</t>
+  </si>
+  <si>
+    <t>BD_EMAIL_5_FIRST</t>
+  </si>
+  <si>
+    <t>BD_EMAIL_5_LAST</t>
+  </si>
+  <si>
+    <t>BD_EMAIL_4_LAST</t>
+  </si>
+  <si>
+    <t>BD_EMAIL_4_FIRST</t>
+  </si>
+  <si>
+    <t>BD_EMAIL_3_LAST</t>
+  </si>
+  <si>
+    <t>BD_EMAIL_3_FIRST</t>
+  </si>
+  <si>
+    <t>BD_EMAIL_2_FIRST</t>
+  </si>
+  <si>
+    <t>BD_EMAIL_2_LAST</t>
+  </si>
+  <si>
+    <t>BD_PHONE_2_FIRST</t>
+  </si>
+  <si>
+    <t>BD_PHONE_2_LAST</t>
+  </si>
+  <si>
+    <t>BD_PHONE_3_FIRST</t>
+  </si>
+  <si>
+    <t>BD_PHONE_3_LAST</t>
+  </si>
+  <si>
+    <t>BD_PHONE_4_FIRST</t>
+  </si>
+  <si>
+    <t>BD_PHONE_4_LAST</t>
+  </si>
+  <si>
+    <t>BD_PHONE_5_FIRST</t>
+  </si>
+  <si>
+    <t>BD_PHONE_5_LAST</t>
+  </si>
+  <si>
+    <t>BD_PHONE_6_FIRST</t>
+  </si>
+  <si>
+    <t>BD_PHONE_6_LAST</t>
+  </si>
+  <si>
+    <t>BD_PHONE_7_FIRST</t>
+  </si>
+  <si>
+    <t>BD_PHONE_7_LAST</t>
+  </si>
+  <si>
+    <t>BD_PHONE_8_FIRST</t>
+  </si>
+  <si>
+    <t>BD_PHONE_8_LAST</t>
+  </si>
+  <si>
+    <t>BD_PHONE_9_FIRST</t>
+  </si>
+  <si>
+    <t>BD_PHONE_9_LAST</t>
+  </si>
+  <si>
+    <t>BD_PHONE_10_FIRST</t>
+  </si>
+  <si>
+    <t>BD_PHONE_10_LAST</t>
   </si>
 </sst>
 </file>
@@ -440,7 +560,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -459,8 +579,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -494,11 +626,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -515,26 +660,23 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -864,19 +1006,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F02CFFD2-F536-E04C-865D-01ECD3155642}">
-  <dimension ref="A1:DU8"/>
+  <dimension ref="A1:FI8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="ES1" workbookViewId="0">
+      <selection activeCell="FC8" sqref="FC8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="17" width="17.1640625" style="2" customWidth="1"/>
     <col min="18" max="18" width="16.1640625" style="2" customWidth="1"/>
-    <col min="19" max="117" width="17.1640625" style="2" customWidth="1"/>
-    <col min="118" max="125" width="17.1640625" customWidth="1"/>
+    <col min="19" max="157" width="17.1640625" style="2" customWidth="1"/>
+    <col min="158" max="165" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:125" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:165" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -991,270 +1135,548 @@
       <c r="AL1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AM1" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="AN1" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="AO1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AU1" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="AV1" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="AW1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="BC1" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="BD1" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="BE1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BK1" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="BL1" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="BM1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BO1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BQ1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BR1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BS1" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="BT1" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="BU1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BV1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BW1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BX1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BY1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="BP1" s="1" t="s">
+      <c r="BZ1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="BQ1" s="1" t="s">
+      <c r="CA1" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="CB1" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="CC1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="BR1" s="1" t="s">
+      <c r="CD1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="BS1" s="1" t="s">
+      <c r="CE1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="BT1" s="1" t="s">
+      <c r="CF1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="BU1" s="1" t="s">
+      <c r="CG1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="BV1" s="1" t="s">
+      <c r="CH1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="BW1" s="1" t="s">
+      <c r="CI1" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="CJ1" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="CK1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="BX1" s="1" t="s">
+      <c r="CL1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="BY1" s="1" t="s">
+      <c r="CM1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="BZ1" s="1" t="s">
+      <c r="CN1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="CA1" s="1" t="s">
+      <c r="CO1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="CB1" s="1" t="s">
+      <c r="CP1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="CC1" s="1" t="s">
+      <c r="CQ1" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="CR1" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="CS1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="CD1" s="1" t="s">
+      <c r="CT1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="CE1" s="1" t="s">
+      <c r="CU1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="CF1" s="1" t="s">
+      <c r="CV1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="CG1" s="1" t="s">
+      <c r="CW1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="CH1" s="1" t="s">
+      <c r="CX1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="CI1" s="1" t="s">
+      <c r="CY1" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="CZ1" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="DA1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="CJ1" s="1" t="s">
+      <c r="DB1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="CK1" s="1" t="s">
+      <c r="DC1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="CL1" s="1" t="s">
+      <c r="DD1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="CM1" s="1" t="s">
+      <c r="DE1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="CN1" s="1" t="s">
+      <c r="DF1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="CO1" s="1" t="s">
+      <c r="DG1" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="DH1" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="DI1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="CP1" s="1" t="s">
+      <c r="DJ1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="CQ1" s="1" t="s">
+      <c r="DK1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="CR1" s="1" t="s">
+      <c r="DL1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="CS1" s="1" t="s">
+      <c r="DM1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="CT1" s="1" t="s">
+      <c r="DN1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="CU1" s="1" t="s">
+      <c r="DO1" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="DP1" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="DQ1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="CV1" s="1" t="s">
+      <c r="DR1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="CW1" s="1" t="s">
+      <c r="DS1" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="DT1" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="DU1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="CX1" s="1" t="s">
+      <c r="DV1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="CY1" s="1" t="s">
+      <c r="DW1" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="DX1" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="DY1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="CZ1" s="1" t="s">
+      <c r="DZ1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="DA1" s="1" t="s">
+      <c r="EA1" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="EB1" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="EC1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="DB1" s="1" t="s">
+      <c r="ED1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="DC1" s="1" t="s">
+      <c r="EE1" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="EF1" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="EG1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="DD1" s="1" t="s">
+      <c r="EH1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="DE1" s="1" t="s">
+      <c r="EI1" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="EJ1" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="EK1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="DF1" s="1" t="s">
+      <c r="EL1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="DG1" s="1" t="s">
+      <c r="EM1" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="EN1" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="EO1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="DH1" s="1" t="s">
+      <c r="EP1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="DI1" s="1" t="s">
+      <c r="EQ1" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="ER1" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="ES1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="DJ1" s="1" t="s">
+      <c r="ET1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="DK1" s="1" t="s">
+      <c r="EU1" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="EV1" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="EW1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="DL1" s="1" t="s">
+      <c r="EX1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="DM1" s="1" t="s">
+      <c r="EY1" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="EZ1" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="FA1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="DN1" s="1" t="s">
+      <c r="FB1" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="DO1" s="1" t="s">
+      <c r="FC1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="DP1" s="1" t="s">
+      <c r="FD1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="DQ1" s="1" t="s">
+      <c r="FE1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="DR1" s="1" t="s">
+      <c r="FF1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="DS1" s="1" t="s">
+      <c r="FG1" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="DT1" s="1" t="s">
+      <c r="FH1" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="DU1" s="1" t="s">
+      <c r="FI1" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:125" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:125" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:165" x14ac:dyDescent="0.2">
+      <c r="A2"/>
+      <c r="B2"/>
+      <c r="C2"/>
+      <c r="D2"/>
+      <c r="E2"/>
+      <c r="F2"/>
+      <c r="G2"/>
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
+      <c r="N2"/>
+      <c r="O2"/>
+      <c r="P2"/>
+      <c r="Q2"/>
+      <c r="R2"/>
+      <c r="S2"/>
+      <c r="T2"/>
+      <c r="U2"/>
+      <c r="V2"/>
+      <c r="W2"/>
+      <c r="X2"/>
+      <c r="Y2"/>
+      <c r="Z2"/>
+      <c r="AA2"/>
+      <c r="AB2"/>
+      <c r="AC2"/>
+      <c r="AD2"/>
+      <c r="AE2"/>
+      <c r="AF2"/>
+      <c r="AG2"/>
+      <c r="AH2"/>
+      <c r="AI2"/>
+      <c r="AJ2"/>
+      <c r="AK2"/>
+      <c r="AL2"/>
+      <c r="AM2"/>
+      <c r="AN2"/>
+      <c r="AO2"/>
+      <c r="AP2"/>
+      <c r="AQ2"/>
+      <c r="AR2"/>
+      <c r="AS2"/>
+      <c r="AT2"/>
+      <c r="AU2"/>
+      <c r="AV2"/>
+      <c r="AW2"/>
+      <c r="AX2"/>
+      <c r="AY2"/>
+      <c r="AZ2"/>
+      <c r="BA2"/>
+      <c r="BB2"/>
+      <c r="BC2"/>
+      <c r="BD2"/>
+      <c r="BE2"/>
+      <c r="BF2"/>
+      <c r="BG2"/>
+      <c r="BH2"/>
+      <c r="BI2"/>
+      <c r="BJ2"/>
+      <c r="BK2"/>
+      <c r="BL2"/>
+      <c r="BM2"/>
+      <c r="BN2"/>
+      <c r="BO2"/>
+      <c r="BP2"/>
+      <c r="BQ2"/>
+      <c r="BR2"/>
+      <c r="BS2"/>
+      <c r="BT2"/>
+      <c r="BU2"/>
+      <c r="BV2"/>
+      <c r="BW2"/>
+      <c r="BX2"/>
+      <c r="BY2"/>
+      <c r="BZ2"/>
+      <c r="CA2"/>
+      <c r="CB2"/>
+      <c r="CC2"/>
+      <c r="CD2"/>
+      <c r="CE2"/>
+      <c r="CF2"/>
+      <c r="CG2"/>
+      <c r="CH2"/>
+      <c r="CI2"/>
+      <c r="CJ2"/>
+      <c r="CK2"/>
+      <c r="CL2"/>
+      <c r="CM2"/>
+      <c r="CN2"/>
+      <c r="CO2"/>
+      <c r="CP2"/>
+      <c r="CQ2"/>
+      <c r="CR2"/>
+      <c r="CS2"/>
+      <c r="CT2"/>
+      <c r="CU2"/>
+      <c r="CV2"/>
+      <c r="CW2"/>
+      <c r="CX2"/>
+      <c r="CY2"/>
+      <c r="CZ2"/>
+      <c r="DA2"/>
+      <c r="DB2"/>
+      <c r="DC2"/>
+      <c r="DD2"/>
+      <c r="DE2"/>
+      <c r="DF2"/>
+      <c r="DG2"/>
+      <c r="DH2"/>
+      <c r="DI2"/>
+      <c r="DJ2"/>
+      <c r="DK2"/>
+      <c r="DL2"/>
+      <c r="DM2"/>
+      <c r="DN2"/>
+      <c r="DO2"/>
+      <c r="DP2"/>
+      <c r="DQ2"/>
+      <c r="DR2"/>
+      <c r="DS2"/>
+      <c r="DT2"/>
+      <c r="DU2"/>
+      <c r="DV2"/>
+      <c r="DW2"/>
+      <c r="DX2"/>
+      <c r="DY2"/>
+      <c r="DZ2"/>
+      <c r="EA2"/>
+      <c r="EB2"/>
+      <c r="EC2"/>
+      <c r="ED2"/>
+      <c r="EE2"/>
+      <c r="EF2"/>
+      <c r="EG2"/>
+      <c r="EH2"/>
+      <c r="EI2"/>
+      <c r="EJ2"/>
+      <c r="EK2"/>
+      <c r="EL2"/>
+      <c r="EM2"/>
+      <c r="EN2"/>
+      <c r="EO2"/>
+      <c r="EP2"/>
+      <c r="EQ2"/>
+      <c r="ER2"/>
+      <c r="ES2"/>
+      <c r="ET2"/>
+      <c r="EU2"/>
+      <c r="EV2"/>
+      <c r="EW2"/>
+      <c r="EX2"/>
+      <c r="EY2"/>
+      <c r="EZ2"/>
+      <c r="FA2"/>
+    </row>
+    <row r="3" spans="1:165" x14ac:dyDescent="0.2">
       <c r="R3"/>
       <c r="S3"/>
       <c r="T3"/>
@@ -1355,121 +1777,193 @@
       <c r="DK3"/>
       <c r="DL3"/>
       <c r="DM3"/>
+      <c r="DN3"/>
+      <c r="DO3"/>
+      <c r="DP3"/>
+      <c r="DQ3"/>
+      <c r="DR3"/>
+      <c r="DS3"/>
+      <c r="DT3"/>
+      <c r="DU3"/>
+      <c r="DV3"/>
+      <c r="DW3"/>
+      <c r="DX3"/>
+      <c r="DY3"/>
+      <c r="DZ3"/>
+      <c r="EA3"/>
+      <c r="EB3"/>
+      <c r="EC3"/>
+      <c r="ED3"/>
+      <c r="EE3"/>
+      <c r="EF3"/>
+      <c r="EG3"/>
+      <c r="EH3"/>
+      <c r="EI3"/>
+      <c r="EJ3"/>
+      <c r="EK3"/>
+      <c r="EL3"/>
+      <c r="EM3"/>
+      <c r="EN3"/>
+      <c r="EO3"/>
+      <c r="EP3"/>
+      <c r="EQ3"/>
+      <c r="ER3"/>
+      <c r="ES3"/>
+      <c r="ET3"/>
+      <c r="EU3"/>
+      <c r="EV3"/>
+      <c r="EW3"/>
+      <c r="EX3"/>
+      <c r="EY3"/>
+      <c r="EZ3"/>
+      <c r="FA3"/>
     </row>
-    <row r="5" spans="1:125" x14ac:dyDescent="0.2">
-      <c r="R5" s="6"/>
-      <c r="S5" s="6"/>
-      <c r="T5" s="6"/>
-      <c r="U5" s="6"/>
-      <c r="V5" s="6"/>
-      <c r="W5" s="6"/>
-      <c r="X5" s="6"/>
-      <c r="Y5" s="6"/>
-      <c r="Z5" s="6"/>
-      <c r="AA5" s="6"/>
-      <c r="AB5" s="6"/>
-      <c r="AC5" s="6"/>
-      <c r="AD5" s="6"/>
-      <c r="AE5" s="6"/>
-      <c r="AF5" s="6"/>
-      <c r="AG5" s="6"/>
-      <c r="AH5" s="6"/>
-      <c r="AI5" s="6"/>
-      <c r="AJ5" s="6"/>
-      <c r="AK5" s="6"/>
-      <c r="AL5" s="6"/>
-      <c r="AM5" s="6"/>
-      <c r="AN5" s="6"/>
-      <c r="AO5" s="6"/>
-      <c r="AP5" s="6"/>
-      <c r="AQ5" s="6"/>
-      <c r="AR5" s="6"/>
-      <c r="AS5" s="6"/>
-      <c r="AT5" s="6"/>
-      <c r="AU5" s="6"/>
-      <c r="AV5" s="6"/>
-      <c r="AW5" s="6"/>
-      <c r="AX5" s="6"/>
-      <c r="AY5" s="6"/>
-      <c r="AZ5" s="6"/>
-      <c r="BA5" s="6"/>
-      <c r="BB5" s="6"/>
-      <c r="BC5" s="6"/>
-      <c r="BD5" s="6"/>
-      <c r="BE5" s="6"/>
-      <c r="BF5" s="6"/>
-      <c r="BG5" s="6"/>
-      <c r="BH5" s="6"/>
-      <c r="BI5" s="6"/>
-      <c r="BJ5" s="6"/>
-      <c r="BK5" s="6"/>
-      <c r="BL5" s="6"/>
-      <c r="BM5" s="6"/>
-      <c r="BN5" s="6"/>
-      <c r="BO5" s="6"/>
-      <c r="BP5" s="6"/>
-      <c r="BQ5" s="6"/>
-      <c r="BR5" s="6"/>
-      <c r="BS5" s="6"/>
-      <c r="BT5" s="6"/>
-      <c r="BU5" s="6"/>
-      <c r="BV5" s="6"/>
-      <c r="BW5" s="6"/>
-      <c r="BX5" s="6"/>
-      <c r="BY5" s="6"/>
-      <c r="BZ5" s="6"/>
-      <c r="CA5" s="6"/>
-      <c r="CB5" s="6"/>
-      <c r="CC5" s="6"/>
-      <c r="CD5" s="6"/>
-      <c r="CE5" s="6"/>
-      <c r="CF5" s="6"/>
-      <c r="CG5" s="6"/>
-      <c r="CH5" s="6"/>
-      <c r="CI5" s="6"/>
-      <c r="CJ5" s="6"/>
-      <c r="CK5" s="6"/>
-      <c r="CL5" s="6"/>
-      <c r="CM5" s="6"/>
-      <c r="CN5" s="6"/>
-      <c r="CO5" s="6"/>
-      <c r="CP5" s="6"/>
-      <c r="CQ5" s="6"/>
-      <c r="CR5" s="6"/>
-      <c r="CS5" s="6"/>
-      <c r="CT5" s="6"/>
-      <c r="CU5" s="6"/>
-      <c r="CV5" s="6"/>
-      <c r="CW5" s="6"/>
-      <c r="CX5" s="6"/>
-      <c r="CY5" s="6"/>
-      <c r="CZ5" s="6"/>
-      <c r="DA5" s="6"/>
-      <c r="DB5" s="6"/>
-      <c r="DC5" s="6"/>
-      <c r="DD5" s="6"/>
-      <c r="DE5" s="6"/>
-      <c r="DF5" s="6"/>
-      <c r="DG5" s="6"/>
-      <c r="DH5" s="6"/>
-      <c r="DI5" s="6"/>
-      <c r="DJ5" s="6"/>
-      <c r="DK5" s="6"/>
-      <c r="DL5" s="6"/>
-      <c r="DM5" s="6"/>
-      <c r="DN5" s="6"/>
-      <c r="DO5" s="6"/>
-      <c r="DP5" s="6"/>
-      <c r="DQ5" s="6"/>
-      <c r="DR5" s="6"/>
-      <c r="DS5" s="6"/>
-      <c r="DT5" s="6"/>
-      <c r="DU5" s="6"/>
+    <row r="5" spans="1:165" x14ac:dyDescent="0.2">
+      <c r="R5"/>
+      <c r="S5"/>
+      <c r="T5"/>
+      <c r="U5"/>
+      <c r="V5"/>
+      <c r="W5"/>
+      <c r="X5"/>
+      <c r="Y5"/>
+      <c r="Z5"/>
+      <c r="AA5"/>
+      <c r="AB5"/>
+      <c r="AC5"/>
+      <c r="AD5"/>
+      <c r="AE5"/>
+      <c r="AF5"/>
+      <c r="AG5"/>
+      <c r="AH5"/>
+      <c r="AI5"/>
+      <c r="AJ5"/>
+      <c r="AK5"/>
+      <c r="AL5"/>
+      <c r="AM5"/>
+      <c r="AN5"/>
+      <c r="AO5"/>
+      <c r="AP5"/>
+      <c r="AQ5"/>
+      <c r="AR5"/>
+      <c r="AS5"/>
+      <c r="AT5"/>
+      <c r="AU5"/>
+      <c r="AV5"/>
+      <c r="AW5"/>
+      <c r="AX5"/>
+      <c r="AY5"/>
+      <c r="AZ5"/>
+      <c r="BA5"/>
+      <c r="BB5"/>
+      <c r="BC5"/>
+      <c r="BD5"/>
+      <c r="BE5"/>
+      <c r="BF5"/>
+      <c r="BG5"/>
+      <c r="BH5"/>
+      <c r="BI5"/>
+      <c r="BJ5"/>
+      <c r="BK5"/>
+      <c r="BL5"/>
+      <c r="BM5"/>
+      <c r="BN5"/>
+      <c r="BO5"/>
+      <c r="BP5"/>
+      <c r="BQ5"/>
+      <c r="BR5"/>
+      <c r="BS5"/>
+      <c r="BT5"/>
+      <c r="BU5"/>
+      <c r="BV5"/>
+      <c r="BW5"/>
+      <c r="BX5"/>
+      <c r="BY5"/>
+      <c r="BZ5"/>
+      <c r="CA5"/>
+      <c r="CB5"/>
+      <c r="CC5"/>
+      <c r="CD5"/>
+      <c r="CE5"/>
+      <c r="CF5"/>
+      <c r="CG5"/>
+      <c r="CH5"/>
+      <c r="CI5"/>
+      <c r="CJ5"/>
+      <c r="CK5"/>
+      <c r="CL5"/>
+      <c r="CM5"/>
+      <c r="CN5"/>
+      <c r="CO5"/>
+      <c r="CP5"/>
+      <c r="CQ5"/>
+      <c r="CR5"/>
+      <c r="CS5"/>
+      <c r="CT5"/>
+      <c r="CU5"/>
+      <c r="CV5"/>
+      <c r="CW5"/>
+      <c r="CX5"/>
+      <c r="CY5"/>
+      <c r="CZ5"/>
+      <c r="DA5"/>
+      <c r="DB5"/>
+      <c r="DC5"/>
+      <c r="DD5"/>
+      <c r="DE5"/>
+      <c r="DF5"/>
+      <c r="DG5"/>
+      <c r="DH5"/>
+      <c r="DI5"/>
+      <c r="DJ5"/>
+      <c r="DK5"/>
+      <c r="DL5"/>
+      <c r="DM5"/>
+      <c r="DN5"/>
+      <c r="DO5"/>
+      <c r="DP5"/>
+      <c r="DQ5"/>
+      <c r="DR5"/>
+      <c r="DS5"/>
+      <c r="DT5"/>
+      <c r="DU5"/>
+      <c r="DV5"/>
+      <c r="DW5"/>
+      <c r="DX5"/>
+      <c r="DY5"/>
+      <c r="DZ5"/>
+      <c r="EA5"/>
+      <c r="EB5"/>
+      <c r="EC5"/>
+      <c r="ED5"/>
+      <c r="EE5"/>
+      <c r="EF5"/>
+      <c r="EG5"/>
+      <c r="EH5"/>
+      <c r="EI5"/>
+      <c r="EJ5"/>
+      <c r="EK5"/>
+      <c r="EL5"/>
+      <c r="EM5"/>
+      <c r="EN5"/>
+      <c r="EO5"/>
+      <c r="EP5"/>
+      <c r="EQ5"/>
+      <c r="ER5"/>
+      <c r="ES5"/>
+      <c r="ET5"/>
+      <c r="EU5"/>
+      <c r="EV5"/>
+      <c r="EW5"/>
+      <c r="EX5"/>
+      <c r="EY5"/>
+      <c r="EZ5"/>
+      <c r="FA5"/>
     </row>
-    <row r="7" spans="1:125" x14ac:dyDescent="0.2">
-      <c r="R7" s="7"/>
+    <row r="7" spans="1:165" x14ac:dyDescent="0.2">
+      <c r="R7" s="6"/>
     </row>
-    <row r="8" spans="1:125" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:165" x14ac:dyDescent="0.2">
       <c r="R8"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Should be working with new Batchdata template now including ECorp to Batch Match Percent field and missing names functionality back and forth for eCorp and BatchData. The new template. I can't really observe these though as the template is still not being processed, so that's what's up next.
</commit_message>
<xml_diff>
--- a/Batchdata_Template.xlsx
+++ b/Batchdata_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrettsullivan/Desktop/BHRF/Data_Recourses/LANDSCRAPE/adhs-working/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28AA11F1-2D83-F140-9505-FD3E8EB6704B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B629EC1E-FEF9-5249-AB6B-3089ED80708F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{ED9AA6DF-8EAD-9141-9DC3-5FD70562401F}"/>
+    <workbookView xWindow="17300" yWindow="0" windowWidth="18540" windowHeight="22400" xr2:uid="{ED9AA6DF-8EAD-9141-9DC3-5FD70562401F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="173">
   <si>
     <t>ECORP_INDEX_#</t>
   </si>
@@ -116,9 +116,6 @@
     <t>BD_SOURCE_ENTITY_ID</t>
   </si>
   <si>
-    <t>BD_TITLE_ROLE</t>
-  </si>
-  <si>
     <t>BD_TARGET_FIRST_NAME</t>
   </si>
   <si>
@@ -531,6 +528,33 @@
   </si>
   <si>
     <t>BD_PHONE_10_LAST</t>
+  </si>
+  <si>
+    <t>ECORP_TO_BATCH_MATCH_%</t>
+  </si>
+  <si>
+    <t>MISSING_1_FULL_NAME</t>
+  </si>
+  <si>
+    <t>MISSING_2_FULL_NAME</t>
+  </si>
+  <si>
+    <t>MISSING_3_FULL_NAME</t>
+  </si>
+  <si>
+    <t>MISSING_4_FULL_NAME</t>
+  </si>
+  <si>
+    <t>MISSING_5_FULL_NAME</t>
+  </si>
+  <si>
+    <t>MISSING_6_FULL_NAME</t>
+  </si>
+  <si>
+    <t>MISSING_7_FULL_NAME</t>
+  </si>
+  <si>
+    <t>MISSING_8_FULL_NAME</t>
   </si>
 </sst>
 </file>
@@ -560,18 +584,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -643,7 +661,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -651,25 +669,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1006,70 +1021,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F02CFFD2-F536-E04C-865D-01ECD3155642}">
-  <dimension ref="A1:FI8"/>
+  <dimension ref="A1:FQ8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="ES1" workbookViewId="0">
-      <selection activeCell="FC8" sqref="FC8"/>
+    <sheetView tabSelected="1" topLeftCell="FJ1" workbookViewId="0">
+      <selection activeCell="FP6" sqref="FP6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="17" width="17.1640625" style="2" customWidth="1"/>
     <col min="18" max="18" width="16.1640625" style="2" customWidth="1"/>
-    <col min="19" max="157" width="17.1640625" style="2" customWidth="1"/>
-    <col min="158" max="165" width="17.1640625" customWidth="1"/>
+    <col min="19" max="156" width="17.1640625" style="2" customWidth="1"/>
+    <col min="157" max="164" width="17.1640625" customWidth="1"/>
+    <col min="165" max="165" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:165" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:173" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="P1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="R1" s="1" t="s">
@@ -1084,7 +1100,7 @@
       <c r="U1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="V1" s="1" t="s">
         <v>26</v>
       </c>
       <c r="W1" s="1" t="s">
@@ -1100,22 +1116,22 @@
         <v>30</v>
       </c>
       <c r="AA1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF1" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="AG1" s="1" t="s">
         <v>32</v>
@@ -1132,14 +1148,14 @@
       <c r="AK1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AL1" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="AM1" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="AN1" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="AM1" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="AN1" s="7" t="s">
-        <v>126</v>
       </c>
       <c r="AO1" s="1" t="s">
         <v>38</v>
@@ -1156,14 +1172,14 @@
       <c r="AS1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AT1" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="AU1" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="AV1" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="AU1" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="AV1" s="7" t="s">
-        <v>148</v>
       </c>
       <c r="AW1" s="1" t="s">
         <v>44</v>
@@ -1180,14 +1196,14 @@
       <c r="BA1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BB1" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="BC1" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="BD1" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="BC1" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="BD1" s="7" t="s">
-        <v>150</v>
       </c>
       <c r="BE1" s="1" t="s">
         <v>50</v>
@@ -1204,14 +1220,14 @@
       <c r="BI1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BJ1" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="BK1" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="BL1" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="BK1" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="BL1" s="7" t="s">
-        <v>152</v>
       </c>
       <c r="BM1" s="1" t="s">
         <v>56</v>
@@ -1228,14 +1244,14 @@
       <c r="BQ1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="BR1" s="1" t="s">
+      <c r="BR1" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="BS1" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="BT1" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="BS1" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="BT1" s="7" t="s">
-        <v>154</v>
       </c>
       <c r="BU1" s="1" t="s">
         <v>62</v>
@@ -1252,14 +1268,14 @@
       <c r="BY1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="BZ1" s="1" t="s">
+      <c r="BZ1" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="CA1" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="CB1" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="CA1" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="CB1" s="7" t="s">
-        <v>156</v>
       </c>
       <c r="CC1" s="1" t="s">
         <v>68</v>
@@ -1276,14 +1292,14 @@
       <c r="CG1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="CH1" s="1" t="s">
+      <c r="CH1" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="CI1" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="CJ1" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="CI1" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="CJ1" s="7" t="s">
-        <v>158</v>
       </c>
       <c r="CK1" s="1" t="s">
         <v>74</v>
@@ -1300,14 +1316,14 @@
       <c r="CO1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="CP1" s="1" t="s">
+      <c r="CP1" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="CQ1" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="CR1" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="CQ1" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="CR1" s="7" t="s">
-        <v>160</v>
       </c>
       <c r="CS1" s="1" t="s">
         <v>80</v>
@@ -1324,14 +1340,14 @@
       <c r="CW1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="CX1" s="1" t="s">
+      <c r="CX1" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="CY1" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="CZ1" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="CY1" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="CZ1" s="7" t="s">
-        <v>162</v>
       </c>
       <c r="DA1" s="1" t="s">
         <v>86</v>
@@ -1348,14 +1364,14 @@
       <c r="DE1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="DF1" s="1" t="s">
+      <c r="DF1" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="DG1" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="DH1" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="DG1" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="DH1" s="7" t="s">
-        <v>164</v>
       </c>
       <c r="DI1" s="1" t="s">
         <v>92</v>
@@ -1372,122 +1388,122 @@
       <c r="DM1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="DN1" s="1" t="s">
+      <c r="DN1" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="DO1" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="DP1" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="DO1" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="DP1" s="7" t="s">
-        <v>128</v>
       </c>
       <c r="DQ1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="DR1" s="1" t="s">
+      <c r="DR1" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="DS1" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="DT1" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="DS1" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="DT1" s="7" t="s">
-        <v>146</v>
       </c>
       <c r="DU1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="DV1" s="1" t="s">
+      <c r="DV1" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="DW1" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="DX1" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="DW1" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="DX1" s="9" t="s">
-        <v>143</v>
       </c>
       <c r="DY1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="DZ1" s="1" t="s">
+      <c r="DZ1" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="EA1" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="EB1" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="EA1" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="EB1" s="9" t="s">
-        <v>141</v>
       </c>
       <c r="EC1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="ED1" s="1" t="s">
-        <v>105</v>
+      <c r="ED1" s="7" t="s">
+        <v>138</v>
       </c>
       <c r="EE1" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="EF1" s="9" t="s">
-        <v>140</v>
+      <c r="EF1" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="EG1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="EH1" s="1" t="s">
-        <v>107</v>
+      <c r="EH1" s="7" t="s">
+        <v>136</v>
       </c>
       <c r="EI1" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="EJ1" s="9" t="s">
-        <v>138</v>
+      <c r="EJ1" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="EK1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="EL1" s="1" t="s">
+      <c r="EL1" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="EM1" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="EN1" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="EM1" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="EN1" s="9" t="s">
-        <v>135</v>
       </c>
       <c r="EO1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="EP1" s="1" t="s">
-        <v>111</v>
+      <c r="EP1" s="7" t="s">
+        <v>132</v>
       </c>
       <c r="EQ1" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="ER1" s="9" t="s">
-        <v>134</v>
+      <c r="ER1" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="ES1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="ET1" s="1" t="s">
-        <v>113</v>
+      <c r="ET1" s="7" t="s">
+        <v>130</v>
       </c>
       <c r="EU1" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="EV1" s="9" t="s">
-        <v>132</v>
+      <c r="EV1" s="1" t="s">
+        <v>113</v>
       </c>
       <c r="EW1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="EX1" s="1" t="s">
-        <v>115</v>
+      <c r="EX1" s="7" t="s">
+        <v>128</v>
       </c>
       <c r="EY1" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="EZ1" s="9" t="s">
-        <v>130</v>
+      <c r="EZ1" s="1" t="s">
+        <v>115</v>
       </c>
       <c r="FA1" s="1" t="s">
         <v>116</v>
@@ -1513,11 +1529,35 @@
       <c r="FH1" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="FI1" s="1" t="s">
-        <v>124</v>
+      <c r="FI1" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="FJ1" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="FK1" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="FL1" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="FM1" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="FN1" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="FO1" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="FP1" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="FQ1" s="2" t="s">
+        <v>172</v>
       </c>
     </row>
-    <row r="2" spans="1:165" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:173" x14ac:dyDescent="0.2">
       <c r="A2"/>
       <c r="B2"/>
       <c r="C2"/>
@@ -1674,9 +1714,8 @@
       <c r="EX2"/>
       <c r="EY2"/>
       <c r="EZ2"/>
-      <c r="FA2"/>
     </row>
-    <row r="3" spans="1:165" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:173" x14ac:dyDescent="0.2">
       <c r="R3"/>
       <c r="S3"/>
       <c r="T3"/>
@@ -1816,9 +1855,8 @@
       <c r="EX3"/>
       <c r="EY3"/>
       <c r="EZ3"/>
-      <c r="FA3"/>
     </row>
-    <row r="5" spans="1:165" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:173" x14ac:dyDescent="0.2">
       <c r="R5"/>
       <c r="S5"/>
       <c r="T5"/>
@@ -1958,12 +1996,11 @@
       <c r="EX5"/>
       <c r="EY5"/>
       <c r="EZ5"/>
-      <c r="FA5"/>
     </row>
-    <row r="7" spans="1:165" x14ac:dyDescent="0.2">
-      <c r="R7" s="6"/>
+    <row r="7" spans="1:173" x14ac:dyDescent="0.2">
+      <c r="R7" s="5"/>
     </row>
-    <row r="8" spans="1:165" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:173" x14ac:dyDescent="0.2">
       <c r="R8"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: improve historical file selection & fix movement case formatting
- process_months_local.py: Select largest file from most recent month
  for historical data (more complete vs test/failed runs)
- analysis.py: Change movement values to Title Case per v300Track_this.md
  (Increased, Decreased, No movement)
- Update Excel templates (Batchdata, Ecorp, v300Dialer)
- Add planning docs (last1percent-plan, analysis-records-dup, GSREALTY)
- gitignore: Add git-nov/ to exclude CleanShot screenshots

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Batchdata_Template.xlsx
+++ b/Batchdata_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrettsullivan/Desktop/BHRF/Data_Recourses/LANDSCRAPE/adhs-working/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78947620-DA63-064B-9CA2-0E5450EB12C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9BA9529-EBCE-A846-83AB-8D34D51C7CEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18040" yWindow="0" windowWidth="17800" windowHeight="22400" xr2:uid="{ED9AA6DF-8EAD-9141-9DC3-5FD70562401F}"/>
+    <workbookView xWindow="18040" yWindow="500" windowWidth="17800" windowHeight="21900" xr2:uid="{ED9AA6DF-8EAD-9141-9DC3-5FD70562401F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="170">
   <si>
     <t>ECORP_INDEX_#</t>
   </si>
@@ -543,6 +543,9 @@
   </si>
   <si>
     <t>MISSING_8_FULL_NAME</t>
+  </si>
+  <si>
+    <t>BATCH_ECORP_CALL_TYPE</t>
   </si>
 </sst>
 </file>
@@ -572,7 +575,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -595,6 +598,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -649,7 +658,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -673,6 +682,9 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1009,22 +1021,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F02CFFD2-F536-E04C-865D-01ECD3155642}">
-  <dimension ref="A1:FM8"/>
+  <dimension ref="A1:FN8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="W7" sqref="W7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="17" width="17.1640625" style="2" customWidth="1"/>
-    <col min="18" max="18" width="16.1640625" style="2" customWidth="1"/>
-    <col min="19" max="152" width="17.1640625" style="2" customWidth="1"/>
-    <col min="153" max="160" width="17.1640625" customWidth="1"/>
-    <col min="161" max="161" width="17.5" customWidth="1"/>
+    <col min="1" max="18" width="17.1640625" style="2" customWidth="1"/>
+    <col min="19" max="19" width="16.1640625" style="2" customWidth="1"/>
+    <col min="20" max="153" width="17.1640625" style="2" customWidth="1"/>
+    <col min="154" max="161" width="17.1640625" customWidth="1"/>
+    <col min="162" max="162" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:169" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:170" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -1076,464 +1088,467 @@
       <c r="Q1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="6" t="s">
+      <c r="AI1" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="AI1" s="6" t="s">
+      <c r="AJ1" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AP1" s="6" t="s">
+      <c r="AQ1" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="AQ1" s="6" t="s">
+      <c r="AR1" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AX1" s="6" t="s">
+      <c r="AY1" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="AY1" s="6" t="s">
+      <c r="AZ1" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="BF1" s="6" t="s">
+      <c r="BG1" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="BG1" s="6" t="s">
+      <c r="BH1" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="BN1" s="6" t="s">
+      <c r="BO1" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="BO1" s="6" t="s">
+      <c r="BP1" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="BP1" s="1" t="s">
+      <c r="BQ1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="BQ1" s="1" t="s">
+      <c r="BR1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="BR1" s="1" t="s">
+      <c r="BS1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="BS1" s="1" t="s">
+      <c r="BT1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="BT1" s="1" t="s">
+      <c r="BU1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="BU1" s="1" t="s">
+      <c r="BV1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="BV1" s="6" t="s">
+      <c r="BW1" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="BW1" s="6" t="s">
+      <c r="BX1" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="BX1" s="1" t="s">
+      <c r="BY1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="BY1" s="1" t="s">
+      <c r="BZ1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="BZ1" s="1" t="s">
+      <c r="CA1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="CA1" s="1" t="s">
+      <c r="CB1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="CB1" s="1" t="s">
+      <c r="CC1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="CC1" s="1" t="s">
+      <c r="CD1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="CD1" s="6" t="s">
+      <c r="CE1" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="CE1" s="6" t="s">
+      <c r="CF1" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="CF1" s="1" t="s">
+      <c r="CG1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="CG1" s="1" t="s">
+      <c r="CH1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="CH1" s="1" t="s">
+      <c r="CI1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="CI1" s="1" t="s">
+      <c r="CJ1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="CJ1" s="1" t="s">
+      <c r="CK1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="CK1" s="1" t="s">
+      <c r="CL1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="CL1" s="6" t="s">
+      <c r="CM1" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="CM1" s="6" t="s">
+      <c r="CN1" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="CN1" s="1" t="s">
+      <c r="CO1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="CO1" s="1" t="s">
+      <c r="CP1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="CP1" s="1" t="s">
+      <c r="CQ1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="CQ1" s="1" t="s">
+      <c r="CR1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="CR1" s="1" t="s">
+      <c r="CS1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="CS1" s="1" t="s">
+      <c r="CT1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="CT1" s="6" t="s">
+      <c r="CU1" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="CU1" s="6" t="s">
+      <c r="CV1" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="CV1" s="1" t="s">
+      <c r="CW1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="CW1" s="1" t="s">
+      <c r="CX1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="CX1" s="1" t="s">
+      <c r="CY1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="CY1" s="1" t="s">
+      <c r="CZ1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="CZ1" s="1" t="s">
+      <c r="DA1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="DA1" s="1" t="s">
+      <c r="DB1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="DB1" s="6" t="s">
+      <c r="DC1" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="DC1" s="6" t="s">
+      <c r="DD1" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="DD1" s="1" t="s">
+      <c r="DE1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="DE1" s="1" t="s">
+      <c r="DF1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="DF1" s="1" t="s">
+      <c r="DG1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="DG1" s="1" t="s">
+      <c r="DH1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="DH1" s="1" t="s">
+      <c r="DI1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="DI1" s="1" t="s">
+      <c r="DJ1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="DJ1" s="6" t="s">
+      <c r="DK1" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="DK1" s="6" t="s">
+      <c r="DL1" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="DL1" s="1" t="s">
+      <c r="DM1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="DM1" s="1" t="s">
+      <c r="DN1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="DN1" s="6" t="s">
+      <c r="DO1" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="DO1" s="6" t="s">
+      <c r="DP1" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="DP1" s="1" t="s">
+      <c r="DQ1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="DQ1" s="1" t="s">
+      <c r="DR1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="DR1" s="7" t="s">
+      <c r="DS1" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="DS1" s="8" t="s">
+      <c r="DT1" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="DT1" s="1" t="s">
+      <c r="DU1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="DU1" s="1" t="s">
+      <c r="DV1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="DV1" s="7" t="s">
+      <c r="DW1" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="DW1" s="8" t="s">
+      <c r="DX1" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="DX1" s="1" t="s">
+      <c r="DY1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="DY1" s="1" t="s">
+      <c r="DZ1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="DZ1" s="7" t="s">
+      <c r="EA1" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="EA1" s="8" t="s">
+      <c r="EB1" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="EB1" s="1" t="s">
+      <c r="EC1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="EC1" s="1" t="s">
+      <c r="ED1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="ED1" s="7" t="s">
+      <c r="EE1" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="EE1" s="8" t="s">
+      <c r="EF1" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="EF1" s="1" t="s">
+      <c r="EG1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="EG1" s="1" t="s">
+      <c r="EH1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="EH1" s="7" t="s">
+      <c r="EI1" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="EI1" s="8" t="s">
+      <c r="EJ1" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="EJ1" s="1" t="s">
+      <c r="EK1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="EK1" s="1" t="s">
+      <c r="EL1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="EL1" s="7" t="s">
+      <c r="EM1" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="EM1" s="8" t="s">
+      <c r="EN1" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="EN1" s="1" t="s">
+      <c r="EO1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="EO1" s="1" t="s">
+      <c r="EP1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="EP1" s="7" t="s">
+      <c r="EQ1" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="EQ1" s="8" t="s">
+      <c r="ER1" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="ER1" s="1" t="s">
+      <c r="ES1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="ES1" s="1" t="s">
+      <c r="ET1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="ET1" s="7" t="s">
+      <c r="EU1" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="EU1" s="8" t="s">
+      <c r="EV1" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="EV1" s="1" t="s">
+      <c r="EW1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="EW1" s="1" t="s">
+      <c r="EX1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="EX1" s="1" t="s">
+      <c r="EY1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="EY1" s="1" t="s">
+      <c r="EZ1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="EZ1" s="1" t="s">
+      <c r="FA1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="FA1" s="1" t="s">
+      <c r="FB1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="FB1" s="1" t="s">
+      <c r="FC1" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="FC1" s="1" t="s">
+      <c r="FD1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="FD1" s="1" t="s">
+      <c r="FE1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="FE1" s="2" t="s">
+      <c r="FF1" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="FF1" s="2" t="s">
+      <c r="FG1" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="FG1" s="2" t="s">
+      <c r="FH1" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="FH1" s="2" t="s">
+      <c r="FI1" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="FI1" s="2" t="s">
+      <c r="FJ1" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="FJ1" s="2" t="s">
+      <c r="FK1" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="FK1" s="2" t="s">
+      <c r="FL1" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="FL1" s="2" t="s">
+      <c r="FM1" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="FM1" s="2" t="s">
+      <c r="FN1" s="2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:169" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:170" x14ac:dyDescent="0.2">
       <c r="A2"/>
       <c r="B2"/>
       <c r="C2"/>
@@ -1686,9 +1701,9 @@
       <c r="ET2"/>
       <c r="EU2"/>
       <c r="EV2"/>
+      <c r="EW2"/>
     </row>
-    <row r="3" spans="1:169" x14ac:dyDescent="0.2">
-      <c r="R3"/>
+    <row r="3" spans="1:170" x14ac:dyDescent="0.2">
       <c r="S3"/>
       <c r="T3"/>
       <c r="U3"/>
@@ -1823,9 +1838,9 @@
       <c r="ET3"/>
       <c r="EU3"/>
       <c r="EV3"/>
+      <c r="EW3"/>
     </row>
-    <row r="5" spans="1:169" x14ac:dyDescent="0.2">
-      <c r="R5"/>
+    <row r="5" spans="1:170" x14ac:dyDescent="0.2">
       <c r="S5"/>
       <c r="T5"/>
       <c r="U5"/>
@@ -1960,12 +1975,13 @@
       <c r="ET5"/>
       <c r="EU5"/>
       <c r="EV5"/>
+      <c r="EW5"/>
     </row>
-    <row r="7" spans="1:169" x14ac:dyDescent="0.2">
-      <c r="R7" s="5"/>
+    <row r="7" spans="1:170" x14ac:dyDescent="0.2">
+      <c r="S7" s="5"/>
     </row>
-    <row r="8" spans="1:169" x14ac:dyDescent="0.2">
-      <c r="R8"/>
+    <row r="8" spans="1:170" x14ac:dyDescent="0.2">
+      <c r="S8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>